<commit_message>
Data Driven Testing with Excel sheet and @DataProvider
</commit_message>
<xml_diff>
--- a/src/main/resources/coursecontent/CourseContent.xlsx
+++ b/src/main/resources/coursecontent/CourseContent.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SARTHAK FOLDERS\PnT Automation_Weekend_Sep_Nov_2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarth\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F218B1-7B1C-4EB2-B57C-26364068DC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3EFD84B-145A-4DFB-A421-9E6B08DFE64A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{EACD1DD4-3EA4-4962-8AD1-9B1A4058DFBF}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{EACD1DD4-3EA4-4962-8AD1-9B1A4058DFBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>Java</t>
   </si>
@@ -365,6 +365,9 @@
   <si>
     <t>main() method in java
 control statements in java</t>
+  </si>
+  <si>
+    <t>Properties file</t>
   </si>
 </sst>
 </file>
@@ -482,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -508,6 +511,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,23 +826,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{328EF461-0BD0-4C99-8C84-ACBA26C6EB5C}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="21" x14ac:dyDescent="0.65"/>
   <cols>
-    <col min="1" max="1" width="49.5234375" style="1" customWidth="1"/>
-    <col min="2" max="3" width="47.26171875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.7890625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="42.68359375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="24.5234375" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.83984375" style="1"/>
+    <col min="1" max="1" width="49.53125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="47.265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="37.796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="42.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="24.53125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.86328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="38.700000000000003" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="38.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -858,7 +862,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A2" s="10" t="s">
         <v>4</v>
       </c>
@@ -878,14 +882,14 @@
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="11" t="s">
         <v>56</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -898,7 +902,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A4" s="10" t="s">
         <v>6</v>
       </c>
@@ -918,7 +922,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="147" customHeight="1" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:6" ht="147" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A5" s="12" t="s">
         <v>105</v>
       </c>
@@ -938,7 +942,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="40.799999999999997" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:6" ht="42" x14ac:dyDescent="0.65">
       <c r="A6" s="13" t="s">
         <v>106</v>
       </c>
@@ -958,14 +962,14 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A7" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="11" t="s">
         <v>60</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -978,7 +982,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A8" s="14" t="s">
         <v>8</v>
       </c>
@@ -998,7 +1002,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
@@ -1018,7 +1022,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -1032,21 +1036,21 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="11" t="s">
         <v>64</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A12" s="6" t="s">
         <v>12</v>
       </c>
@@ -1060,7 +1064,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A13" s="6" t="s">
         <v>13</v>
       </c>
@@ -1074,7 +1078,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
@@ -1088,21 +1092,21 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A15" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="11" t="s">
         <v>68</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.65">
       <c r="A16" s="6" t="s">
         <v>17</v>
       </c>
@@ -1116,46 +1120,46 @@
         <v>93</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A17" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="11" t="s">
         <v>70</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.65">
       <c r="A18" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="11" t="s">
         <v>71</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.65">
       <c r="B19" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="11" t="s">
         <v>72</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.65">
       <c r="B20" s="7" t="s">
         <v>46</v>
       </c>
@@ -1163,7 +1167,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.65">
       <c r="B21" s="7" t="s">
         <v>47</v>
       </c>
@@ -1171,7 +1175,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.65">
       <c r="B22" s="7" t="s">
         <v>48</v>
       </c>
@@ -1179,7 +1183,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.65">
       <c r="B23" s="7" t="s">
         <v>49</v>
       </c>
@@ -1187,7 +1191,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.65">
       <c r="B24" s="7" t="s">
         <v>50</v>
       </c>
@@ -1195,29 +1199,34 @@
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.65">
       <c r="B25" s="7" t="s">
         <v>51</v>
       </c>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.65">
       <c r="B26" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.65">
       <c r="B27" s="7" t="s">
         <v>53</v>
       </c>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.65">
       <c r="B28" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.65">
+      <c r="B29" s="15" t="s">
+        <v>107</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>